<commit_message>
updated structure of analysis notebooks and result exports
</commit_message>
<xml_diff>
--- a/experiments/2021_scientific_reports/results/statistics/stats_cortisol_features.xlsx
+++ b/experiments/2021_scientific_reports/results/statistics/stats_cortisol_features.xlsx
@@ -863,7 +863,7 @@
         <v>0.04137711560838741</v>
       </c>
       <c r="K5">
-        <v>-0.8216466978391058</v>
+        <v>-0.8216466978391057</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -933,7 +933,7 @@
         <v>0.02398918445441276</v>
       </c>
       <c r="K7">
-        <v>-0.8865652473158667</v>
+        <v>-0.8865652473158669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>